<commit_message>
write query in dbcon, arrange data per requirements
</commit_message>
<xml_diff>
--- a/downloads/CurrentInventory.xlsx
+++ b/downloads/CurrentInventory.xlsx
@@ -22,16 +22,16 @@
     <t>Product</t>
   </si>
   <si>
+    <t>L</t>
+  </si>
+  <si>
     <t>M</t>
   </si>
   <si>
+    <t>S</t>
+  </si>
+  <si>
     <t>XL</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>S</t>
   </si>
   <si>
     <t>XS</t>
@@ -375,13 +375,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,7 +404,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -412,49 +412,22 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E2">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>30</v>
       </c>
       <c r="G2">
-        <v>30</v>
-      </c>
-      <c r="H2">
-        <v>15</v>
-      </c>
-      <c r="I2">
-        <v>12</v>
-      </c>
-      <c r="J2">
-        <v>30</v>
-      </c>
-      <c r="K2">
-        <v>40</v>
-      </c>
-      <c r="L2">
         <v>22</v>
       </c>
-      <c r="M2">
-        <v>35</v>
-      </c>
-      <c r="N2">
-        <v>30</v>
-      </c>
-      <c r="O2">
-        <v>30</v>
-      </c>
-      <c r="P2">
-        <v>30</v>
-      </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -462,15 +435,12 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D3">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="F3">
         <v>24</v>
       </c>
     </row>

</xml_diff>